<commit_message>
Integrating Exel utility into the framework
</commit_message>
<xml_diff>
--- a/PythonSelFramework/PythonDemo.xlsx
+++ b/PythonSelFramework/PythonDemo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\Python\AUTOMATION\Framework\PythonSelFramework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8D300C-E37A-484B-A8B9-E46348D15D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621904BF-A1F1-4AB9-800A-A684AB03532C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5280" yWindow="3375" windowWidth="21600" windowHeight="11385" xr2:uid="{7C37AF48-BD68-4F69-88AE-A57AA707953B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -116,6 +116,24 @@
   </si>
   <si>
     <t>Lopes</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>search</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>iphone X</t>
+  </si>
+  <si>
+    <t>United</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
   </si>
 </sst>
 </file>
@@ -484,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38B64A5D-F988-4BB2-915A-113A3B45AB67}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,9 +514,10 @@
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -514,8 +533,17 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -532,7 +560,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -549,24 +577,21 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>85</v>
-      </c>
-      <c r="D4">
-        <v>57</v>
-      </c>
-      <c r="E4">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -583,7 +608,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -600,7 +625,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -617,7 +642,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -634,7 +659,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -651,7 +676,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -668,7 +693,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -685,7 +710,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -702,7 +727,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -719,7 +744,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -736,7 +761,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>

</xml_diff>